<commit_message>
Updated EmployeeServiceClient to get service params from Excel doc. Updated test_config.json to set the webservice_host_url and EmployeeSericeClient to use it.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Employees/Employees.xlsx
+++ b/src/test/resources/testdata/Employees/Employees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waterfall\IdeaProjects\udbdpd\src\test\resources\testdata\Employees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4D5C6D-A4F2-4E4D-A42F-6FC85F52D7F5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AC29B7-33CC-46E1-802E-FEBAC0199B96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="5623" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Feature File</t>
   </si>
@@ -174,12 +174,6 @@
     <t>[employeeName]</t>
   </si>
   <si>
-    <t>Parameter Key</t>
-  </si>
-  <si>
-    <t>Parameter Value</t>
-  </si>
-  <si>
     <t>employeeName</t>
   </si>
   <si>
@@ -190,6 +184,9 @@
   </si>
   <si>
     <t>/api/empdb/employee</t>
+  </si>
+  <si>
+    <t>failed</t>
   </si>
 </sst>
 </file>
@@ -766,10 +763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAD1096-CA41-46A1-AD31-33408DCA0C75}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -779,10 +776,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -790,7 +787,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -798,14 +795,6 @@
         <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>